<commit_message>
View All Med View Specific Med Submit Repl Req
</commit_message>
<xml_diff>
--- a/data/Medicine_List.xlsx
+++ b/data/Medicine_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2024S1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiachun/IdeaProjects/SC2002_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C048B4EB-70E3-47B1-AB1B-763235055723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0FD81B-166C-A94D-B107-F06C3A1197C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,17 +408,17 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -440,18 +440,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added approve replenish page
</commit_message>
<xml_diff>
--- a/data/Medicine_List.xlsx
+++ b/data/Medicine_List.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiachun/IdeaProjects/SC2002_Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\IdeaProjects\SC2002_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0FD81B-166C-A94D-B107-F06C3A1197C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{3C46459D-6343-4638-B200-8975E3F33165}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Medicine Name</t>
   </si>
@@ -38,12 +38,19 @@
   </si>
   <si>
     <t>Amoxicillin</t>
+  </si>
+  <si>
+    <t>CCure</t>
+  </si>
+  <si>
+    <t>CC7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,19 +101,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -123,10 +130,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -284,7 +291,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -293,13 +300,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -309,7 +316,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -318,7 +325,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -327,7 +334,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -337,12 +344,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -373,7 +380,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -392,7 +399,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -404,21 +411,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -440,18 +447,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -462,7 +469,29 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>470.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added: View presc record Added: Update presc status Fixed: Allignment for the Views
</commit_message>
<xml_diff>
--- a/data/Medicine_List.xlsx
+++ b/data/Medicine_List.xlsx
@@ -440,8 +440,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>100</v>
+      <c r="B2" t="n">
+        <v>98.0</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -451,8 +451,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>50</v>
+      <c r="B3" t="n">
+        <v>47.0</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -462,8 +462,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>75</v>
+      <c r="B4" t="n">
+        <v>73.0</v>
       </c>
       <c r="C4">
         <v>15</v>

</xml_diff>

<commit_message>
Shifted UpdatePrescriptionScreen Fixed Outcomeloader
</commit_message>
<xml_diff>
--- a/data/Medicine_List.xlsx
+++ b/data/Medicine_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Medicine Name</t>
   </si>
@@ -441,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>98.0</v>
+        <v>91.0</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -452,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>47.0</v>
+        <v>46.0</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -463,7 +463,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>73.0</v>
+        <v>72.0</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -485,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>470.0</v>
+        <v>478.0</v>
       </c>
       <c r="C6" t="n">
         <v>10.0</v>

</xml_diff>